<commit_message>
netcdf common variable options
</commit_message>
<xml_diff>
--- a/meta-data/surface-met.xlsx
+++ b/meta-data/surface-met.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CC4675-33B9-414C-AC51-E98159ADF489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3E57B-6343-9448-9111-52B589751801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5040" windowWidth="17360" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="17360" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="105">
   <si>
     <t>units</t>
   </si>
@@ -358,24 +358,6 @@
   </si>
   <si>
     <t>Surface brightness temperature (9.6-11.5 um) at the Met Mast (heated window)</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>degrees longitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>degrees latitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
   </si>
   <si>
     <t>qc_flag_skin_temperature_1</t>
@@ -833,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:F1086"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2847,7 +2829,7 @@
     <row r="281" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="282" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A282" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B282" s="3"/>
       <c r="C282" s="13"/>
@@ -2885,7 +2867,7 @@
         <v>14</v>
       </c>
       <c r="C286" s="16" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="287" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2909,7 +2891,7 @@
     <row r="289" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="290" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A290" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B290" s="3"/>
       <c r="C290" s="13"/>
@@ -2947,7 +2929,7 @@
         <v>14</v>
       </c>
       <c r="C294" s="16" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2973,177 +2955,29 @@
       <c r="B297" s="17"/>
       <c r="C297" s="18"/>
     </row>
-    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A298" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B299" t="s">
-        <v>8</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B300" t="s">
-        <v>10</v>
-      </c>
-      <c r="C300" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B301" t="s">
-        <v>0</v>
-      </c>
-      <c r="C301" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B302" t="s">
-        <v>13</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B303" t="s">
-        <v>14</v>
-      </c>
-      <c r="C303" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B304" t="s">
-        <v>16</v>
-      </c>
-      <c r="C304" s="4">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B305" t="s">
-        <v>17</v>
-      </c>
-      <c r="C305" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B306" t="s">
-        <v>19</v>
-      </c>
-      <c r="C306" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B307" t="s">
-        <v>20</v>
-      </c>
-      <c r="C307" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B308" t="s">
-        <v>22</v>
-      </c>
-      <c r="C308" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A310" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B311" t="s">
-        <v>8</v>
-      </c>
-      <c r="C311" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B312" t="s">
-        <v>10</v>
-      </c>
-      <c r="C312" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B313" t="s">
-        <v>0</v>
-      </c>
-      <c r="C313" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B314" t="s">
-        <v>13</v>
-      </c>
-      <c r="C314" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B315" t="s">
-        <v>14</v>
-      </c>
-      <c r="C315" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B316" t="s">
-        <v>16</v>
-      </c>
-      <c r="C316" s="4">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B317" t="s">
-        <v>17</v>
-      </c>
-      <c r="C317" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B318" t="s">
-        <v>19</v>
-      </c>
-      <c r="C318" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B319" t="s">
-        <v>20</v>
-      </c>
-      <c r="C319" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B320" t="s">
-        <v>22</v>
-      </c>
-      <c r="C320" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="321" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="322" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="323" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add valid min and max to skin temperature variable
</commit_message>
<xml_diff>
--- a/meta-data/surface-met.xlsx
+++ b/meta-data/surface-met.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3E57B-6343-9448-9111-52B589751801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9FCEE-DA35-B94C-B0B4-897AB66DF88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1040" windowWidth="17360" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="105">
   <si>
     <t>units</t>
   </si>
@@ -813,10 +813,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1086"/>
+  <dimension ref="A1:F1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="C299" sqref="C299"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2209,756 +2209,784 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B190" t="s">
+        <v>17</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="13" t="s">
+      <c r="B191" t="s">
+        <v>19</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C191" s="13"/>
-    </row>
-    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B192" t="s">
-        <v>8</v>
-      </c>
-      <c r="C192" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B193" t="s">
-        <v>10</v>
-      </c>
-      <c r="C193" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="C193" s="13"/>
     </row>
     <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B194" t="s">
-        <v>0</v>
-      </c>
-      <c r="C194" s="13" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B195" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C195" s="13" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B196" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B197" t="s">
-        <v>16</v>
-      </c>
-      <c r="C197" s="14">
-        <v>-1E+20</v>
+        <v>14</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B198" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C198" s="13" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B199" t="s">
+        <v>16</v>
+      </c>
+      <c r="C199" s="14">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B200" t="s">
+        <v>20</v>
+      </c>
+      <c r="C200" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B201" t="s">
         <v>22</v>
       </c>
-      <c r="C199" s="13" t="s">
+      <c r="C201" s="13" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B202" t="s">
-        <v>8</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>46</v>
+        <v>17</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B203" t="s">
-        <v>10</v>
-      </c>
-      <c r="C203" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B204" t="s">
-        <v>0</v>
-      </c>
-      <c r="C204" s="8">
-        <v>1</v>
-      </c>
-    </row>
+        <v>19</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B205" t="s">
-        <v>13</v>
-      </c>
-      <c r="C205" s="8"/>
+      <c r="A205" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B206" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B207" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B208" t="s">
+        <v>0</v>
+      </c>
+      <c r="C208" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B209" t="s">
+        <v>13</v>
+      </c>
+      <c r="C209" s="8"/>
+    </row>
+    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B210" t="s">
         <v>14</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C210" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B207" s="6" t="s">
+    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B211" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C207" s="9" t="s">
+      <c r="C211" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B208" s="10" t="s">
+    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B212" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C208" s="11" t="s">
+      <c r="C212" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" t="s">
+    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B211" t="s">
-        <v>8</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B212" t="s">
-        <v>10</v>
-      </c>
-      <c r="C212" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B213" t="s">
-        <v>0</v>
-      </c>
-      <c r="C213" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B214" t="s">
-        <v>13</v>
-      </c>
-      <c r="C214" s="8"/>
     </row>
     <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B215" t="s">
+        <v>8</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B216" t="s">
+        <v>10</v>
+      </c>
+      <c r="C216" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B217" t="s">
+        <v>0</v>
+      </c>
+      <c r="C217" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B218" t="s">
+        <v>13</v>
+      </c>
+      <c r="C218" s="8"/>
+    </row>
+    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B219" t="s">
         <v>14</v>
       </c>
-      <c r="C215" s="3" t="s">
+      <c r="C219" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B216" s="6" t="s">
+    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B220" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C216" s="9" t="s">
+      <c r="C220" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B217" s="10" t="s">
+    <row r="221" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B221" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C217" s="11" t="s">
+      <c r="C221" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" t="s">
+    <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A223" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B220" t="s">
-        <v>8</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B221" t="s">
-        <v>10</v>
-      </c>
-      <c r="C221" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C222" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B223" t="s">
-        <v>13</v>
-      </c>
-      <c r="C223" s="8"/>
     </row>
     <row r="224" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B224" t="s">
+        <v>8</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B225" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B226" t="s">
+        <v>0</v>
+      </c>
+      <c r="C226" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B227" t="s">
+        <v>13</v>
+      </c>
+      <c r="C227" s="8"/>
+    </row>
+    <row r="228" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B228" t="s">
         <v>14</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C228" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B225" s="6" t="s">
+    <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B229" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C225" s="9" t="s">
+      <c r="C229" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B226" s="10" t="s">
+    <row r="230" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B230" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C226" s="11" t="s">
+      <c r="C230" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="3" t="s">
+    <row r="231" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A232" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B229" t="s">
-        <v>8</v>
-      </c>
-      <c r="C229" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B230" t="s">
-        <v>10</v>
-      </c>
-      <c r="C230" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B231" t="s">
-        <v>0</v>
-      </c>
-      <c r="C231" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B232" t="s">
-        <v>13</v>
-      </c>
-      <c r="C232" s="8"/>
     </row>
     <row r="233" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B233" t="s">
+        <v>8</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B234" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B235" t="s">
+        <v>0</v>
+      </c>
+      <c r="C235" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B236" t="s">
+        <v>13</v>
+      </c>
+      <c r="C236" s="8"/>
+    </row>
+    <row r="237" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B237" t="s">
         <v>14</v>
       </c>
-      <c r="C233" s="3" t="s">
+      <c r="C237" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B234" s="6" t="s">
+    <row r="238" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B238" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C234" s="9" t="s">
+      <c r="C238" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B235" s="10" t="s">
+    <row r="239" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B239" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C235" s="18" t="s">
+      <c r="C239" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A237" s="3" t="s">
+    <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A241" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B238" t="s">
-        <v>8</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B239" t="s">
-        <v>10</v>
-      </c>
-      <c r="C239" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B240" t="s">
-        <v>0</v>
-      </c>
-      <c r="C240" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B241" t="s">
-        <v>13</v>
-      </c>
-      <c r="C241" s="8"/>
     </row>
     <row r="242" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B242" t="s">
+        <v>8</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B243" t="s">
+        <v>10</v>
+      </c>
+      <c r="C243" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B244" t="s">
+        <v>0</v>
+      </c>
+      <c r="C244" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B245" t="s">
+        <v>13</v>
+      </c>
+      <c r="C245" s="8"/>
+    </row>
+    <row r="246" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B246" t="s">
         <v>14</v>
       </c>
-      <c r="C242" s="3" t="s">
+      <c r="C246" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B243" s="6" t="s">
+    <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B247" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C243" s="9" t="s">
+      <c r="C247" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B244" s="10" t="s">
+    <row r="248" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B248" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C244" s="11" t="s">
+      <c r="C248" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A246" s="12" t="s">
+    <row r="249" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A250" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B247" t="s">
-        <v>8</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B248" t="s">
-        <v>10</v>
-      </c>
-      <c r="C248" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B249" t="s">
-        <v>0</v>
-      </c>
-      <c r="C249" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B250" t="s">
-        <v>13</v>
-      </c>
-      <c r="C250" s="8"/>
     </row>
     <row r="251" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B251" t="s">
+        <v>8</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B252" t="s">
+        <v>10</v>
+      </c>
+      <c r="C252" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B253" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B254" t="s">
+        <v>13</v>
+      </c>
+      <c r="C254" s="8"/>
+    </row>
+    <row r="255" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B255" t="s">
         <v>14</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C255" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B252" s="6" t="s">
+    <row r="256" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B256" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C252" s="9" t="s">
+      <c r="C256" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B253" s="10" t="s">
+    <row r="257" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B257" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C253" s="18" t="s">
+      <c r="C257" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A255" s="12" t="s">
+    <row r="258" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A259" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B256" t="s">
-        <v>8</v>
-      </c>
-      <c r="C256" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B257" t="s">
-        <v>10</v>
-      </c>
-      <c r="C257" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B258" t="s">
-        <v>0</v>
-      </c>
-      <c r="C258" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B259" t="s">
-        <v>13</v>
-      </c>
-      <c r="C259" s="8"/>
     </row>
     <row r="260" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B260" t="s">
+        <v>8</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B261" t="s">
+        <v>10</v>
+      </c>
+      <c r="C261" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B262" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B263" t="s">
+        <v>13</v>
+      </c>
+      <c r="C263" s="8"/>
+    </row>
+    <row r="264" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B264" t="s">
         <v>14</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C264" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B261" s="6" t="s">
+    <row r="265" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B265" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C261" s="9" t="s">
+      <c r="C265" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B262" s="10" t="s">
+    <row r="266" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B266" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C262" s="18" t="s">
+      <c r="C266" s="18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B263" s="10"/>
-      <c r="C263" s="11"/>
-    </row>
-    <row r="264" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A264" s="12" t="s">
+    <row r="267" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B267" s="10"/>
+      <c r="C267" s="11"/>
+    </row>
+    <row r="268" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A268" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B265" t="s">
-        <v>8</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B266" t="s">
-        <v>10</v>
-      </c>
-      <c r="C266" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B267" t="s">
-        <v>0</v>
-      </c>
-      <c r="C267" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B268" t="s">
-        <v>13</v>
-      </c>
-      <c r="C268" s="8"/>
     </row>
     <row r="269" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B269" t="s">
+        <v>8</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B270" t="s">
+        <v>10</v>
+      </c>
+      <c r="C270" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B271" t="s">
+        <v>0</v>
+      </c>
+      <c r="C271" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B272" t="s">
+        <v>13</v>
+      </c>
+      <c r="C272" s="8"/>
+    </row>
+    <row r="273" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B273" t="s">
         <v>14</v>
       </c>
-      <c r="C269" s="12" t="s">
+      <c r="C273" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B270" s="6" t="s">
+    <row r="274" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B274" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C270" s="9" t="s">
+      <c r="C274" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B271" s="10" t="s">
+    <row r="275" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B275" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C271" s="18" t="s">
+      <c r="C275" s="18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B272" s="10"/>
-      <c r="C272" s="11"/>
-    </row>
-    <row r="273" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A273" s="12" t="s">
+    <row r="276" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B276" s="10"/>
+      <c r="C276" s="11"/>
+    </row>
+    <row r="277" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A277" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B274" t="s">
-        <v>8</v>
-      </c>
-      <c r="C274" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B275" t="s">
-        <v>10</v>
-      </c>
-      <c r="C275" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B276" t="s">
-        <v>0</v>
-      </c>
-      <c r="C276" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B277" t="s">
-        <v>13</v>
-      </c>
-      <c r="C277" s="8"/>
     </row>
     <row r="278" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B278" t="s">
+        <v>8</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B279" t="s">
+        <v>10</v>
+      </c>
+      <c r="C279" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B280" t="s">
+        <v>0</v>
+      </c>
+      <c r="C280" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B281" t="s">
+        <v>13</v>
+      </c>
+      <c r="C281" s="8"/>
+    </row>
+    <row r="282" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B282" t="s">
         <v>14</v>
       </c>
-      <c r="C278" s="12" t="s">
+      <c r="C282" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B279" s="6" t="s">
+    <row r="283" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B283" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C279" s="9" t="s">
+      <c r="C283" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B280" s="10" t="s">
+    <row r="284" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B284" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C280" s="18" t="s">
+      <c r="C284" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A282" s="15" t="s">
+    <row r="285" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A286" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B282" s="3"/>
-      <c r="C282" s="13"/>
-    </row>
-    <row r="283" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A283" s="3"/>
-      <c r="B283" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C283" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A284" s="3"/>
-      <c r="B284" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C284" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A285" s="3"/>
-      <c r="B285" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C285" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A286" s="3"/>
-      <c r="B286" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C286" s="16" t="s">
-        <v>103</v>
-      </c>
+      <c r="B286" s="3"/>
+      <c r="C286" s="13"/>
     </row>
     <row r="287" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3"/>
       <c r="B287" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C287" s="9" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="C287" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A288" s="3"/>
-      <c r="B288" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C288" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="B288" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C288" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A289" s="3"/>
+      <c r="B289" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" s="13">
+        <v>1</v>
+      </c>
+    </row>
     <row r="290" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A290" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B290" s="3"/>
-      <c r="C290" s="13"/>
+      <c r="A290" s="3"/>
+      <c r="B290" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C290" s="16" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="291" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3"/>
       <c r="B291" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C291" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C291" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3"/>
-      <c r="B292" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C292" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A293" s="3"/>
-      <c r="B293" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C293" s="13">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B292" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C292" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="294" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A294" s="3"/>
-      <c r="B294" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C294" s="16" t="s">
-        <v>104</v>
-      </c>
+      <c r="A294" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B294" s="3"/>
+      <c r="C294" s="13"/>
     </row>
     <row r="295" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A295" s="3"/>
       <c r="B295" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C295" s="9" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="C295" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="296" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="3"/>
-      <c r="B296" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C296" s="18" t="s">
-        <v>78</v>
+      <c r="B296" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C296" s="13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="3"/>
-      <c r="B297" s="17"/>
-      <c r="C297" s="18"/>
-    </row>
-    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="B297" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C297" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A298" s="3"/>
+      <c r="B298" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C298" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A299" s="3"/>
+      <c r="B299" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C299" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A300" s="3"/>
+      <c r="B300" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C300" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A301" s="3"/>
+      <c r="B301" s="17"/>
+      <c r="C301" s="18"/>
+    </row>
     <row r="302" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="303" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="304" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3744,6 +3772,10 @@
     <row r="1084" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1085" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1086" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1087" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1088" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1089" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1090" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove qc standard names
</commit_message>
<xml_diff>
--- a/meta-data/surface-met.xlsx
+++ b/meta-data/surface-met.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9FCEE-DA35-B94C-B0B4-897AB66DF88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88B7E25-E4B6-8A4B-9C86-641D46164240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1040" windowWidth="17360" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="105">
   <si>
     <t>units</t>
   </si>
@@ -279,9 +279,6 @@
     <t>snow_temperature</t>
   </si>
   <si>
-    <t>qc_snow_temperature</t>
-  </si>
-  <si>
     <t>Data Quality flag: Snow temperature</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
   </si>
   <si>
     <t>Ice to snow heat flux</t>
-  </si>
-  <si>
-    <t>qc_ice_to_snow_heat_flux</t>
   </si>
   <si>
     <t>Data Quality flag: Ice to snow heat flux</t>
@@ -370,6 +364,12 @@
   </si>
   <si>
     <t>Data Quality flag: Skin Temperature  (Radiometer stand)</t>
+  </si>
+  <si>
+    <t>qc_flag_snow_temperature</t>
+  </si>
+  <si>
+    <t>qc_flag_ice_to_snow_heat_flux</t>
   </si>
 </sst>
 </file>
@@ -813,10 +813,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1090"/>
+  <dimension ref="A1:F1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D202" sqref="D202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209:XFD209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1896,7 +1896,7 @@
     <row r="146" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="147" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1928,7 +1928,7 @@
         <v>13</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E151" s="3"/>
     </row>
@@ -1937,7 +1937,7 @@
         <v>14</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1999,7 +1999,7 @@
         <v>10</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2024,7 +2024,7 @@
         <v>14</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2070,7 +2070,7 @@
     <row r="170" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="171" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A171" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2086,7 +2086,7 @@
         <v>10</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2102,7 +2102,7 @@
         <v>13</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E175" s="3"/>
     </row>
@@ -2111,7 +2111,7 @@
         <v>14</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2141,7 +2141,7 @@
     <row r="180" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C181" s="13"/>
     </row>
@@ -2174,7 +2174,7 @@
         <v>14</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2228,7 +2228,7 @@
     <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C193" s="13"/>
     </row>
@@ -2261,7 +2261,7 @@
         <v>14</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2344,439 +2344,448 @@
     </row>
     <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B209" t="s">
-        <v>13</v>
-      </c>
-      <c r="C209" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="C209" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B210" t="s">
-        <v>14</v>
-      </c>
-      <c r="C210" t="s">
-        <v>47</v>
+      <c r="B210" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B211" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C211" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B212" s="10" t="s">
+      <c r="B211" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C212" s="11" t="s">
+      <c r="C211" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" t="s">
-        <v>52</v>
+      <c r="B214" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B215" t="s">
-        <v>8</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>46</v>
+        <v>10</v>
+      </c>
+      <c r="C215" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B216" t="s">
-        <v>10</v>
-      </c>
-      <c r="C216" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="C216" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B217" t="s">
-        <v>0</v>
-      </c>
-      <c r="C217" s="8">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B218" t="s">
-        <v>13</v>
-      </c>
-      <c r="C218" s="8"/>
+      <c r="B218" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B219" t="s">
-        <v>14</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B220" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C220" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
+      <c r="B219" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C219" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="221" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B221" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C221" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="A221" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B222" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A223" t="s">
-        <v>56</v>
+      <c r="B223" t="s">
+        <v>10</v>
+      </c>
+      <c r="C223" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B224" t="s">
-        <v>8</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
+      </c>
+      <c r="C224" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B225" t="s">
+        <v>14</v>
+      </c>
+      <c r="C225" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B226" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B227" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C227" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A229" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B230" t="s">
+        <v>8</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B231" t="s">
         <v>10</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C231" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B226" t="s">
+    <row r="232" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B232" t="s">
         <v>0</v>
       </c>
-      <c r="C226" s="8">
+      <c r="C232" s="8">
         <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B227" t="s">
-        <v>13</v>
-      </c>
-      <c r="C227" s="8"/>
-    </row>
-    <row r="228" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B228" t="s">
-        <v>14</v>
-      </c>
-      <c r="C228" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B229" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C229" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B230" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C230" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B233" t="s">
+        <v>14</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B234" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B235" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C235" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A237" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B238" t="s">
         <v>8</v>
       </c>
-      <c r="C233" s="3" t="s">
+      <c r="C238" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B234" t="s">
+    <row r="239" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B239" t="s">
         <v>10</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C239" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B235" t="s">
+    <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B240" t="s">
         <v>0</v>
       </c>
-      <c r="C235" s="8">
+      <c r="C240" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B236" t="s">
-        <v>13</v>
-      </c>
-      <c r="C236" s="8"/>
-    </row>
-    <row r="237" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B237" t="s">
+    <row r="241" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B241" t="s">
         <v>14</v>
       </c>
-      <c r="C237" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B238" s="6" t="s">
+      <c r="C241" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B242" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C238" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B239" s="10" t="s">
+      <c r="C242" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B243" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C239" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A241" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B242" t="s">
-        <v>8</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B243" t="s">
-        <v>10</v>
-      </c>
-      <c r="C243" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B244" t="s">
-        <v>0</v>
-      </c>
-      <c r="C244" s="8">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="C243" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="245" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B245" t="s">
-        <v>13</v>
-      </c>
-      <c r="C245" s="8"/>
+      <c r="A245" s="12" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="246" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B246" t="s">
+        <v>8</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B247" t="s">
+        <v>10</v>
+      </c>
+      <c r="C247" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B248" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B249" t="s">
         <v>14</v>
       </c>
-      <c r="C246" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B247" s="6" t="s">
+      <c r="C249" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B250" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C247" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B248" s="10" t="s">
+      <c r="C250" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B251" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C248" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A250" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B251" t="s">
-        <v>8</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B252" t="s">
-        <v>10</v>
-      </c>
-      <c r="C252" t="s">
-        <v>11</v>
-      </c>
-    </row>
+      <c r="C251" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="253" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B253" t="s">
-        <v>0</v>
-      </c>
-      <c r="C253" s="8">
-        <v>1</v>
+      <c r="A253" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B254" t="s">
-        <v>13</v>
-      </c>
-      <c r="C254" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="255" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B255" t="s">
+        <v>10</v>
+      </c>
+      <c r="C255" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B256" t="s">
+        <v>0</v>
+      </c>
+      <c r="C256" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B257" t="s">
         <v>14</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C257" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B256" s="6" t="s">
+    <row r="258" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B258" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C256" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B257" s="10" t="s">
+      <c r="C258" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B259" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C257" s="18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A259" s="12" t="s">
-        <v>75</v>
+      <c r="C259" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B260" t="s">
-        <v>8</v>
-      </c>
-      <c r="C260" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="B260" s="10"/>
+      <c r="C260" s="11"/>
     </row>
     <row r="261" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B261" t="s">
-        <v>10</v>
-      </c>
-      <c r="C261" t="s">
-        <v>11</v>
+      <c r="A261" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B262" t="s">
-        <v>0</v>
-      </c>
-      <c r="C262" s="8">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B263" t="s">
-        <v>13</v>
-      </c>
-      <c r="C263" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="C263" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="264" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B264" t="s">
+        <v>0</v>
+      </c>
+      <c r="C264" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B265" t="s">
         <v>14</v>
       </c>
-      <c r="C264" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B265" s="6" t="s">
+      <c r="C265" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B266" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C265" s="9" t="s">
+      <c r="C266" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B267" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C267" s="18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B266" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C266" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B267" s="10"/>
-      <c r="C267" s="11"/>
-    </row>
     <row r="268" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A268" s="12" t="s">
-        <v>86</v>
-      </c>
+      <c r="B268" s="10"/>
+      <c r="C268" s="11"/>
     </row>
     <row r="269" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B269" t="s">
-        <v>8</v>
-      </c>
-      <c r="C269" s="3" t="s">
-        <v>46</v>
+      <c r="A269" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B270" t="s">
-        <v>10</v>
-      </c>
-      <c r="C270" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B271" t="s">
-        <v>0</v>
-      </c>
-      <c r="C271" s="8">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C271" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B272" t="s">
-        <v>13</v>
-      </c>
-      <c r="C272" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="C272" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="273" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B273" t="s">
         <v>14</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2784,7 +2793,7 @@
         <v>48</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2792,201 +2801,147 @@
         <v>50</v>
       </c>
       <c r="C275" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B276" s="10"/>
-      <c r="C276" s="11"/>
-    </row>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="277" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A277" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A277" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B277" s="3"/>
+      <c r="C277" s="13"/>
     </row>
     <row r="278" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B278" t="s">
+      <c r="A278" s="3"/>
+      <c r="B278" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C278" s="3" t="s">
+      <c r="C278" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B279" t="s">
+      <c r="A279" s="3"/>
+      <c r="B279" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C279" t="s">
+      <c r="C279" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B280" t="s">
+      <c r="A280" s="3"/>
+      <c r="B280" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C280" s="8">
+      <c r="C280" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B281" t="s">
-        <v>13</v>
-      </c>
-      <c r="C281" s="8"/>
+      <c r="A281" s="3"/>
+      <c r="B281" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C281" s="16" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="282" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B282" t="s">
-        <v>14</v>
-      </c>
-      <c r="C282" s="12" t="s">
-        <v>81</v>
+      <c r="A282" s="3"/>
+      <c r="B282" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C282" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B283" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C283" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B284" s="10" t="s">
+      <c r="A283" s="3"/>
+      <c r="B283" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C284" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="C283" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A285" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B285" s="3"/>
+      <c r="C285" s="13"/>
+    </row>
     <row r="286" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A286" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B286" s="3"/>
-      <c r="C286" s="13"/>
+      <c r="A286" s="3"/>
+      <c r="B286" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C286" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="287" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3"/>
       <c r="B287" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C287" s="13" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A288" s="3"/>
       <c r="B288" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C288" s="13" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="C288" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A289" s="3"/>
       <c r="B289" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C289" s="13">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C289" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A290" s="3"/>
       <c r="B290" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C290" s="16" t="s">
-        <v>103</v>
+        <v>48</v>
+      </c>
+      <c r="C290" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3"/>
-      <c r="B291" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C291" s="9" t="s">
-        <v>77</v>
+      <c r="B291" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C291" s="18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3"/>
-      <c r="B292" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C292" s="18" t="s">
-        <v>78</v>
-      </c>
+      <c r="B292" s="17"/>
+      <c r="C292" s="18"/>
     </row>
     <row r="293" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A294" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B294" s="3"/>
-      <c r="C294" s="13"/>
-    </row>
-    <row r="295" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A295" s="3"/>
-      <c r="B295" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C295" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A296" s="3"/>
-      <c r="B296" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C296" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A297" s="3"/>
-      <c r="B297" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C297" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A298" s="3"/>
-      <c r="B298" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C298" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A299" s="3"/>
-      <c r="B299" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C299" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A300" s="3"/>
-      <c r="B300" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C300" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A301" s="3"/>
-      <c r="B301" s="17"/>
-      <c r="C301" s="18"/>
-    </row>
+    <row r="294" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="302" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="303" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="304" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3767,15 +3722,6 @@
     <row r="1079" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1080" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1081" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1082" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1083" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1084" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1085" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1086" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1087" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1088" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1089" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1090" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>